<commit_message>
criado mais opcoes para senhas
</commit_message>
<xml_diff>
--- a/senhas.xlsx
+++ b/senhas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\projeto1devaprender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F435C9-6E87-4B6F-B014-B75FAE661BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64FA6FA-06C7-4BBD-B0E0-71C56D2A539F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="690" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -337,10 +337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,6 +375,16 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>